<commit_message>
Remove usless fields from userImportTemplate
</commit_message>
<xml_diff>
--- a/static/userImportTemplate.xlsx
+++ b/static/userImportTemplate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>phone</t>
-  </si>
-  <si>
-    <t>singleDevice</t>
-  </si>
-  <si>
-    <t>deviceId</t>
   </si>
   <si>
     <t>sdjfs</t>
@@ -166,10 +160,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -197,12 +191,6 @@
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -234,50 +222,50 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>